<commit_message>
Added ExtentConfig.xml file for Extent Reports.
</commit_message>
<xml_diff>
--- a/MasterFramework/src/test/resources/TestData/AutomationTestData.xlsx
+++ b/MasterFramework/src/test/resources/TestData/AutomationTestData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="17">
   <si>
     <t>TCID</t>
   </si>
@@ -64,6 +64,9 @@
   </si>
   <si>
     <t>acid_qa</t>
+  </si>
+  <si>
+    <t>Fail</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Modified code to add information in reports and test runner
</commit_message>
<xml_diff>
--- a/MasterFramework/src/test/resources/TestData/AutomationTestData.xlsx
+++ b/MasterFramework/src/test/resources/TestData/AutomationTestData.xlsx
@@ -4,19 +4,18 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14700" windowHeight="3225" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14700" windowHeight="3225"/>
   </bookViews>
   <sheets>
     <sheet name="TestScenario" sheetId="1" r:id="rId1"/>
     <sheet name="VerifyCRMLogin" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="23">
   <si>
     <t>TCID</t>
   </si>
@@ -57,16 +56,34 @@
     <t>Yes</t>
   </si>
   <si>
+    <t>https://kmb.crmnext.com/sng7/app/login/login</t>
+  </si>
+  <si>
+    <t>acid_qa</t>
+  </si>
+  <si>
+    <t>Module</t>
+  </si>
+  <si>
+    <t>Test Type</t>
+  </si>
+  <si>
+    <t>Leads</t>
+  </si>
+  <si>
+    <t>Sanity</t>
+  </si>
+  <si>
+    <t>TC02</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>Regression</t>
+  </si>
+  <si>
     <t>Pass</t>
-  </si>
-  <si>
-    <t>https://kmb.crmnext.com/sng7/app/login/login</t>
-  </si>
-  <si>
-    <t>acid_qa</t>
-  </si>
-  <si>
-    <t>Fail</t>
   </si>
 </sst>
 </file>
@@ -153,7 +170,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -161,12 +178,63 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -477,10 +545,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -488,10 +556,12 @@
     <col min="1" max="1" customWidth="true" width="11.85546875"/>
     <col min="2" max="2" customWidth="true" width="29.42578125"/>
     <col min="3" max="3" customWidth="true" width="17.85546875"/>
-    <col min="4" max="4" customWidth="true" width="14.28515625"/>
+    <col min="4" max="4" customWidth="true" width="12.140625"/>
+    <col min="5" max="5" customWidth="true" width="12.7109375"/>
+    <col min="6" max="6" customWidth="true" width="14.28515625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -502,10 +572,16 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -515,13 +591,97 @@
       <c r="C2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>13</v>
+      <c r="D2" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:C2">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="8" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C3">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="6" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C4">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="4" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C5">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
     <cfRule type="cellIs" priority="2" operator="equal">
@@ -529,14 +689,18 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C5">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="B2" location="VerifyCRMLogin!A1" display="VerifyCRMLogin"/>
+    <hyperlink ref="B3" location="VerifyCRMLogin!A1" display="VerifyCRMLogin"/>
+    <hyperlink ref="B4" location="VerifyCRMLogin!A1" display="VerifyCRMLogin"/>
+    <hyperlink ref="B5" location="VerifyCRMLogin!A1" display="VerifyCRMLogin"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -544,7 +708,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -579,7 +743,7 @@
         <v>4</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>9</v>
@@ -588,7 +752,7 @@
         <v>10</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changes for extent reports
</commit_message>
<xml_diff>
--- a/MasterFramework/src/test/resources/TestData/AutomationTestData.xlsx
+++ b/MasterFramework/src/test/resources/TestData/AutomationTestData.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="23">
   <si>
     <t>TCID</t>
   </si>
@@ -91,7 +91,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -120,6 +120,13 @@
       <name val="Cambria"/>
       <family val="1"/>
       <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -170,7 +177,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -179,32 +186,15 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="4">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -545,10 +535,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -622,42 +612,30 @@
       </c>
     </row>
     <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>18</v>
-      </c>
+      <c r="A4" s="8"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
     </row>
     <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>21</v>
-      </c>
+      <c r="A5" s="8"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="9"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:C2">
-    <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="7" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
     <cfRule type="cellIs" priority="8" operator="equal">
@@ -665,23 +643,23 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3">
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="5" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
     <cfRule type="cellIs" priority="6" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C4">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+  <conditionalFormatting sqref="B4">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
     <cfRule type="cellIs" priority="4" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C5">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+  <conditionalFormatting sqref="B5">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
     <cfRule type="cellIs" priority="2" operator="equal">
@@ -689,15 +667,13 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:B5 C2:C3">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="B2" location="VerifyCRMLogin!A1" display="VerifyCRMLogin"/>
     <hyperlink ref="B3" location="VerifyCRMLogin!A1" display="VerifyCRMLogin"/>
-    <hyperlink ref="B4" location="VerifyCRMLogin!A1" display="VerifyCRMLogin"/>
-    <hyperlink ref="B5" location="VerifyCRMLogin!A1" display="VerifyCRMLogin"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -709,7 +685,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Standardization of extent reports
</commit_message>
<xml_diff>
--- a/MasterFramework/src/test/resources/TestData/AutomationTestData.xlsx
+++ b/MasterFramework/src/test/resources/TestData/AutomationTestData.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="24">
   <si>
     <t>TCID</t>
   </si>
@@ -84,6 +84,9 @@
   </si>
   <si>
     <t>Pass</t>
+  </si>
+  <si>
+    <t>Fail</t>
   </si>
 </sst>
 </file>

</xml_diff>